<commit_message>
Player Hit State 추가
- Player Projectile 스크립트에 몬스터 hit 추가
- Player Status 수정
- Player Projectile 트윈 수정중
</commit_message>
<xml_diff>
--- a/Assets/StaticData/Excel/PlayerStatus.xlsx
+++ b/Assets/StaticData/Excel/PlayerStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\CoffeeCat_RogueLite_Project\Assets\StaticData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02C9EAB-0632-4180-B07B-312C8D919CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA31A61C-616E-4794-B5D2-B6E60030E622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6870" windowWidth="16440" windowHeight="28320" xr2:uid="{CEFF60A8-3F85-4A92-8727-6613D870E2B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CEFF60A8-3F85-4A92-8727-6613D870E2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,81 +33,140 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HealthPoint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvincibleTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackDelay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProjectileSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackPower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CriticalChance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CriticalResistance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Penetration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FlowerMagician</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hit시 무적시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격 딜레이(높으면 공속↓)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발사체 속도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치명타 확률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치명타 저항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관통력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HealthPoint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Defense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MoveSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvincibleTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AttackDelay</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AttackRange</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProjectileSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AttackPower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CriticalChance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CriticalResistance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Penetration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FlowerMagician</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>인덱스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이름</t>
+    <t>CriticalMultiplier</t>
+  </si>
+  <si>
+    <t>치명타 배율</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 속도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격 범위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대미지 계수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DamageDeviation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -115,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +190,40 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="에스코어 드림 5 Medium"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="에스코어 드림 5 Medium"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,12 +240,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,171 +573,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFB7CDA-B6DD-480D-906E-C7E484E83C4A}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.25" customWidth="1"/>
-    <col min="3" max="3" width="11.625" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="6" max="6" width="13.375" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
-    <col min="9" max="9" width="14.875" customWidth="1"/>
-    <col min="10" max="10" width="12.375" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="16.25" customWidth="1"/>
-    <col min="13" max="13" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
+    <col min="9" max="9" width="16.75" customWidth="1"/>
+    <col min="10" max="10" width="14.25" customWidth="1"/>
+    <col min="11" max="11" width="16.75" customWidth="1"/>
+    <col min="12" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="15" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>15</v>
+      <c r="C4" s="2">
+        <v>100</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="I4" s="1">
-        <v>5</v>
-      </c>
-      <c r="J4" s="1">
-        <v>10</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
+    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>